<commit_message>
Add USART1 and DMA configurations, initialize additional timers
</commit_message>
<xml_diff>
--- a/参考资料/电气连接表.xlsx
+++ b/参考资料/电气连接表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sky\Desktop\MCDP\code\AKS_CAR\参考资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STM32\Aks_SmartCar\Aks-SmartCar\参考资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ECB818-1EEF-4725-93FB-7E34221FA624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6456240-EDDF-4CBD-AEB8-8F27C1964055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{1220A042-B9C9-4738-A05B-507579105497}"/>
+    <workbookView xWindow="4470" yWindow="1750" windowWidth="19200" windowHeight="11170" xr2:uid="{1220A042-B9C9-4738-A05B-507579105497}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="153">
   <si>
     <t>舵机</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -629,6 +629,10 @@
   </si>
   <si>
     <t>PG4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -912,20 +916,122 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -935,108 +1041,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1355,7 +1359,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1373,16 +1377,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1411,22 +1415,22 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="42" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="12" t="s">
@@ -1435,18 +1439,18 @@
       <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="50" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="20"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1459,14 +1463,14 @@
       <c r="B5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="48" t="s">
         <v>117</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="20"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1479,12 +1483,12 @@
       <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="57"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="20"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="12" t="s">
         <v>43</v>
       </c>
@@ -1497,12 +1501,12 @@
       <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="57"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1515,34 +1519,34 @@
       <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="58"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="42" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="12" t="s">
@@ -1551,18 +1555,18 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="50" t="s">
+      <c r="C10" s="55"/>
+      <c r="D10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="20"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="12" t="s">
         <v>12</v>
       </c>
@@ -1575,14 +1579,14 @@
       <c r="B11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="48" t="s">
         <v>117</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="20"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="12" t="s">
         <v>13</v>
       </c>
@@ -1595,12 +1599,12 @@
       <c r="B12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="12" t="s">
         <v>14</v>
       </c>
@@ -1613,12 +1617,12 @@
       <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="12" t="s">
         <v>15</v>
       </c>
@@ -1631,184 +1635,184 @@
       <c r="B14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="58"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="31"/>
-    </row>
-    <row r="16" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36" t="s">
+      <c r="I15" s="38"/>
+    </row>
+    <row r="16" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="36" t="s">
+      <c r="C16" s="57"/>
+      <c r="D16" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="29" t="s">
+      <c r="E16" s="53"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="33"/>
-      <c r="I16" s="31"/>
-    </row>
-    <row r="17" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="H16" s="32"/>
+      <c r="I16" s="38"/>
+    </row>
+    <row r="17" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39" t="s">
+      <c r="E17" s="53"/>
+      <c r="F17" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="36" t="s">
+      <c r="C18" s="57"/>
+      <c r="D18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="29" t="s">
+      <c r="E18" s="53"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="33"/>
-    </row>
-    <row r="19" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39" t="s">
+      <c r="E19" s="53"/>
+      <c r="F19" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="33"/>
-    </row>
-    <row r="20" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="36" t="s">
+      <c r="C20" s="57"/>
+      <c r="D20" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="29" t="s">
+      <c r="E20" s="53"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="33"/>
-    </row>
-    <row r="21" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36" t="s">
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39" t="s">
+      <c r="E21" s="53"/>
+      <c r="F21" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="36" t="s">
+      <c r="H21" s="32"/>
+      <c r="I21" s="38"/>
+    </row>
+    <row r="22" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="36" t="s">
+      <c r="C22" s="57"/>
+      <c r="D22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="29" t="s">
+      <c r="E22" s="53"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="31"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -1817,16 +1821,16 @@
       <c r="B23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="30" t="s">
         <v>117</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="42" t="s">
         <v>2</v>
       </c>
       <c r="G23" s="12" t="s">
@@ -1835,20 +1839,20 @@
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="50" t="s">
+      <c r="D24" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="20"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="12" t="s">
         <v>34</v>
       </c>
@@ -1861,14 +1865,14 @@
       <c r="B25" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="30" t="s">
         <v>117</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="20" t="s">
+      <c r="E25" s="41"/>
+      <c r="F25" s="42" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="12" t="s">
@@ -1877,20 +1881,20 @@
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="50" t="s">
+      <c r="A26" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="D26" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="20"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="12" t="s">
         <v>34</v>
       </c>
@@ -1903,14 +1907,14 @@
       <c r="B27" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="30" t="s">
         <v>117</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="20" t="s">
+      <c r="E27" s="41"/>
+      <c r="F27" s="42" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="12" t="s">
@@ -1919,39 +1923,39 @@
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="20"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="12" t="s">
         <v>34</v>
       </c>
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="43" t="s">
+      <c r="E29" s="45" t="s">
         <v>55</v>
       </c>
       <c r="F29" s="44" t="s">
@@ -1960,45 +1964,45 @@
       <c r="G29" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="42" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="41" t="s">
+      <c r="C30" s="37"/>
+      <c r="D30" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="43"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="44"/>
       <c r="G30" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="20"/>
+      <c r="H30" s="42"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="51" t="s">
+      <c r="D31" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="52" t="s">
+      <c r="E31" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="F31" s="53" t="s">
+      <c r="F31" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="12" t="s">
@@ -2007,20 +2011,20 @@
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="51" t="s">
+      <c r="D32" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="52"/>
-      <c r="F32" s="53" t="s">
+      <c r="E32" s="43"/>
+      <c r="F32" s="28" t="s">
         <v>48</v>
       </c>
       <c r="G32" s="12" t="s">
@@ -2029,46 +2033,46 @@
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="47" t="s">
+      <c r="F33" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H33" s="27"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="28" t="s">
+      <c r="C34" s="35"/>
+      <c r="D34" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="48"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="27" t="s">
+      <c r="E34" s="35"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="H34" s="27"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
@@ -2076,24 +2080,24 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
@@ -2119,11 +2123,19 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="H15:H22"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E15:E22"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="A36:F37"/>
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="F3:F8"/>
@@ -2139,20 +2151,12 @@
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="C5:C8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="E15:E22"/>
+    <mergeCell ref="H15:H22"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I21:I22"/>
     <mergeCell ref="H29:H30"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2181,14 +2185,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -2211,128 +2215,128 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21">
+      <c r="A3" s="41">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="58" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="58"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="58" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="58"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+      <c r="A7" s="41">
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="58" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="58"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="58" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2377,13 +2381,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -2405,7 +2409,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="59" t="s">
         <v>113</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -2417,12 +2421,12 @@
       <c r="D3" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="60" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="14" t="s">
         <v>100</v>
       </c>
@@ -2430,10 +2434,10 @@
         <v>105</v>
       </c>
       <c r="D4" s="14"/>
-      <c r="E4" s="26"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="14" t="s">
         <v>101</v>
       </c>
@@ -2443,7 +2447,7 @@
       <c r="D5" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="60"/>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">

</xml_diff>

<commit_message>
Add TIM7 configuration and update motor feedback functions
</commit_message>
<xml_diff>
--- a/参考资料/电气连接表.xlsx
+++ b/参考资料/电气连接表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STM32\Aks_SmartCar\Aks-SmartCar\参考资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6456240-EDDF-4CBD-AEB8-8F27C1964055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502D7E11-AEC8-407F-9EE3-919000680CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4470" yWindow="1750" windowWidth="19200" windowHeight="11170" xr2:uid="{1220A042-B9C9-4738-A05B-507579105497}"/>
   </bookViews>
@@ -952,6 +952,69 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -961,12 +1024,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -975,63 +1032,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445FF531-B602-45E7-BB41-083D65F73ADF}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1377,16 +1377,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1421,16 +1421,16 @@
       <c r="B3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="37" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="44" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="12" t="s">
@@ -1445,12 +1445,12 @@
       <c r="B4" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1463,14 +1463,14 @@
       <c r="B5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="34" t="s">
         <v>117</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
       <c r="G5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1483,12 +1483,12 @@
       <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="42"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="12" t="s">
         <v>43</v>
       </c>
@@ -1501,12 +1501,12 @@
       <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="49"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1519,12 +1519,12 @@
       <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="50"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="12" t="s">
         <v>16</v>
       </c>
@@ -1537,16 +1537,16 @@
       <c r="B9" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="37" t="s">
         <v>118</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="44" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="12" t="s">
@@ -1561,12 +1561,12 @@
       <c r="B10" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="55"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="12" t="s">
         <v>12</v>
       </c>
@@ -1579,14 +1579,14 @@
       <c r="B11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="34" t="s">
         <v>117</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="12" t="s">
         <v>13</v>
       </c>
@@ -1599,12 +1599,12 @@
       <c r="B12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="44"/>
       <c r="G12" s="12" t="s">
         <v>14</v>
       </c>
@@ -1617,12 +1617,12 @@
       <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="49"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
       <c r="G13" s="12" t="s">
         <v>15</v>
       </c>
@@ -1635,12 +1635,12 @@
       <c r="B14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="50"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
       <c r="G14" s="12" t="s">
         <v>16</v>
       </c>
@@ -1653,25 +1653,25 @@
       <c r="B15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="39" t="s">
         <v>120</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="32" t="s">
         <v>60</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="38"/>
+      <c r="I15" s="57"/>
     </row>
     <row r="16" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
@@ -1680,17 +1680,17 @@
       <c r="B16" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="57"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="52"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="38"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
@@ -1699,20 +1699,20 @@
       <c r="B17" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="39" t="s">
         <v>121</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="52" t="s">
+      <c r="E17" s="33"/>
+      <c r="F17" s="32" t="s">
         <v>61</v>
       </c>
       <c r="G17" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="32"/>
+      <c r="H17" s="53"/>
     </row>
     <row r="18" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
@@ -1721,16 +1721,16 @@
       <c r="B18" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="C18" s="57"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="52"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="32"/>
+      <c r="H18" s="53"/>
     </row>
     <row r="19" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
@@ -1739,20 +1739,20 @@
       <c r="B19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="39" t="s">
         <v>127</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="53"/>
-      <c r="F19" s="52" t="s">
+      <c r="E19" s="33"/>
+      <c r="F19" s="32" t="s">
         <v>62</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="32"/>
+      <c r="H19" s="53"/>
     </row>
     <row r="20" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -1761,16 +1761,16 @@
       <c r="B20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="57"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="53"/>
-      <c r="F20" s="52"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="32"/>
+      <c r="H20" s="53"/>
     </row>
     <row r="21" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -1779,21 +1779,21 @@
       <c r="B21" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="39" t="s">
         <v>126</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="53"/>
-      <c r="F21" s="52" t="s">
+      <c r="E21" s="33"/>
+      <c r="F21" s="32" t="s">
         <v>63</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="38"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="57"/>
     </row>
     <row r="22" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -1802,17 +1802,17 @@
       <c r="B22" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="57"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="52"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="32"/>
       <c r="G22" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H22" s="33"/>
-      <c r="I22" s="38"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -1827,10 +1827,10 @@
       <c r="D23" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="44" t="s">
         <v>2</v>
       </c>
       <c r="G23" s="12" t="s">
@@ -1851,8 +1851,8 @@
       <c r="D24" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
       <c r="G24" s="12" t="s">
         <v>34</v>
       </c>
@@ -1871,8 +1871,8 @@
       <c r="D25" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="42" t="s">
+      <c r="E25" s="43"/>
+      <c r="F25" s="44" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="12" t="s">
@@ -1893,8 +1893,8 @@
       <c r="D26" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="44"/>
       <c r="G26" s="12" t="s">
         <v>34</v>
       </c>
@@ -1913,8 +1913,8 @@
       <c r="D27" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42" t="s">
+      <c r="E27" s="43"/>
+      <c r="F27" s="44" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="12" t="s">
@@ -1935,8 +1935,8 @@
       <c r="D28" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="42"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="44"/>
       <c r="G28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1949,22 +1949,22 @@
       <c r="B29" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="55" t="s">
         <v>136</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="45" t="s">
+      <c r="E29" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="44" t="s">
+      <c r="F29" s="46" t="s">
         <v>54</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="42" t="s">
+      <c r="H29" s="44" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1975,16 +1975,16 @@
       <c r="B30" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="37"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="45"/>
-      <c r="F30" s="44"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="46"/>
       <c r="G30" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="42"/>
+      <c r="H30" s="44"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
@@ -1999,7 +1999,7 @@
       <c r="D31" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="45" t="s">
         <v>0</v>
       </c>
       <c r="F31" s="28" t="s">
@@ -2023,7 +2023,7 @@
       <c r="D32" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="43"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="28" t="s">
         <v>48</v>
       </c>
@@ -2039,16 +2039,16 @@
       <c r="B33" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="48" t="s">
         <v>135</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="50" t="s">
         <v>114</v>
       </c>
       <c r="G33" s="19" t="s">
@@ -2063,12 +2063,12 @@
       <c r="B34" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="35"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="35"/>
-      <c r="F34" s="47"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="51"/>
       <c r="G34" s="19" t="s">
         <v>58</v>
       </c>
@@ -2080,24 +2080,24 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
@@ -2123,19 +2123,10 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="E15:E22"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="H29:H30"/>
     <mergeCell ref="A36:F37"/>
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="F3:F8"/>
@@ -2151,12 +2142,21 @@
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E15:E22"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="H15:H22"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="H29:H30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2185,14 +2185,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -2215,16 +2215,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="41">
+      <c r="A3" s="43">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -2235,26 +2235,26 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
       <c r="E4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="58"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -2265,28 +2265,28 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="58"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="41">
+      <c r="A7" s="43">
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="12" t="s">
@@ -2297,26 +2297,26 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="58"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="12" t="s">
@@ -2327,12 +2327,12 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="12" t="s">
         <v>27</v>
       </c>
@@ -2381,13 +2381,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>

</xml_diff>